<commit_message>
metaphysics of upper classes and properties
</commit_message>
<xml_diff>
--- a/project/excel/beril_model.xlsx
+++ b/project/excel/beril_model.xlsx
@@ -8,8 +8,13 @@
   </bookViews>
   <sheets>
     <sheet name="NamedThing" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Person" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="PersonCollection" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Observation" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="NonProcess" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="MaterialEntity" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="InformationArtifact" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Process" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Person" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="PersonCollection" sheetId="8" state="visible" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -451,6 +456,109 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>raw_value</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>observations</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -462,30 +570,132 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>size_in_bytes</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>md5</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>url</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>inputs</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>outputs</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
           <t>primary_email</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
+          <t>birth_date</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
           <t>age_in_years</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>vital_status</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>id</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
@@ -493,7 +703,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="D2:D1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"ALIVE,DEAD,UNKNOWN"</formula1>
     </dataValidation>
   </dataValidations>
@@ -501,7 +711,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>

</xml_diff>

<commit_message>
collection examples inc DH
</commit_message>
<xml_diff>
--- a/project/excel/beril_model.xlsx
+++ b/project/excel/beril_model.xlsx
@@ -7,14 +7,15 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="NamedThing" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Observation" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="NonProcess" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="MaterialEntity" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="InformationArtifact" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="Process" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="Person" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="PersonCollection" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="NamedThingCollection" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="NamedThing" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Observation" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="NonProcess" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="MaterialEntity" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="SoilSample" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="DnaExtract" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="InformationArtifact" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="Process" sheetId="9" state="visible" r:id="rId9"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -420,7 +421,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -431,17 +432,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>id</t>
+          <t>material_entities</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>description</t>
+          <t>processes</t>
         </is>
       </c>
     </row>
@@ -451,6 +447,47 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>type_value</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -468,42 +505,6 @@
       <c r="A1" t="inlineStr">
         <is>
           <t>raw_value</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>description</t>
         </is>
       </c>
     </row>
@@ -529,22 +530,22 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>observations</t>
+          <t>id</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>id</t>
+          <t>name</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>name</t>
+          <t>description</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>description</t>
+          <t>type_value</t>
         </is>
       </c>
     </row>
@@ -570,36 +571,41 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>size_in_bytes</t>
+          <t>mass_g</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>md5</t>
+          <t>color</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>url</t>
+          <t>id</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>id</t>
+          <t>name</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>name</t>
+          <t>description</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>description</t>
+          <t>type_value</t>
         </is>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"RED,GREEN,BLUE"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -610,7 +616,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -621,12 +627,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>inputs</t>
+          <t>mass_g</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>outputs</t>
+          <t>color</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
@@ -642,15 +648,81 @@
       <c r="E1" t="inlineStr">
         <is>
           <t>description</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>type_value</t>
         </is>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"RED,GREEN,BLUE"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>mass_g</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>color</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>type_value</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"RED,GREEN,BLUE"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -667,57 +739,52 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>primary_email</t>
+          <t>size_in_bytes</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>birth_date</t>
+          <t>md5</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>age_in_years</t>
+          <t>url</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>vital_status</t>
+          <t>id</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>id</t>
+          <t>name</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>name</t>
+          <t>description</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>description</t>
+          <t>type_value</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation sqref="D2:D1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"ALIVE,DEAD,UNKNOWN"</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -728,7 +795,32 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>entries</t>
+          <t>inputs</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>outputs</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>type_value</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
can dump a homogeneous collection
</commit_message>
<xml_diff>
--- a/project/excel/beril_model.xlsx
+++ b/project/excel/beril_model.xlsx
@@ -9,8 +9,8 @@
   <sheets>
     <sheet name="NamedThingCollection" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="NamedThing" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Observation" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="NonProcess" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Person" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="PersonCollection" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="MaterialEntity" sheetId="5" state="visible" r:id="rId5"/>
     <sheet name="SoilSample" sheetId="6" state="visible" r:id="rId6"/>
     <sheet name="DnaExtract" sheetId="7" state="visible" r:id="rId7"/>
@@ -452,7 +452,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,127 +476,112 @@
           <t>description</t>
         </is>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>first_name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>last_name</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>people</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>mass_g</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>color</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>type_value</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>raw_value</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
           <t>name</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>description</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>type_value</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>mass_g</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>color</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>type_value</t>
         </is>
       </c>
     </row>
@@ -616,7 +601,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -648,11 +633,6 @@
       <c r="E1" t="inlineStr">
         <is>
           <t>description</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>type_value</t>
         </is>
       </c>
     </row>
@@ -672,7 +652,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -704,11 +684,6 @@
       <c r="E1" t="inlineStr">
         <is>
           <t>description</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>type_value</t>
         </is>
       </c>
     </row>
@@ -728,7 +703,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -767,11 +742,6 @@
           <t>description</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>type_value</t>
-        </is>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -784,7 +754,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -818,11 +788,6 @@
           <t>description</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>type_value</t>
-        </is>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
fixed beril-model DH Playground link
</commit_message>
<xml_diff>
--- a/project/excel/beril_model.xlsx
+++ b/project/excel/beril_model.xlsx
@@ -16,6 +16,8 @@
     <sheet name="DnaExtract" sheetId="7" state="visible" r:id="rId7"/>
     <sheet name="InformationArtifact" sheetId="8" state="visible" r:id="rId8"/>
     <sheet name="Process" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="Splitting" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="Pooling" sheetId="11" state="visible" r:id="rId11"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -446,6 +448,98 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>inputs</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>outputs</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>inputs</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>outputs</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>